<commit_message>
Customization in tree nodes but not effected.
</commit_message>
<xml_diff>
--- a/public/resources/data/JanAliFamilyDatabase.xlsx
+++ b/public/resources/data/JanAliFamilyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JanAli\janalisinformation\frontend\janaliinformationsystem\public\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32CA9B6-82BD-458A-B901-CF0CD0314D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E42ADC-698C-4294-AAC3-4C32D0F3BE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="110">
   <si>
     <t>Id</t>
   </si>
@@ -343,9 +343,6 @@
     <t>Waliya Batool</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>DOB</t>
   </si>
   <si>
@@ -360,8 +357,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="mmmm\,\ yyyy"/>
-    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmmm\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -432,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,13 +447,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -680,7 +674,7 @@
   <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="104" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G13" sqref="G2:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -699,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -708,13 +702,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -752,9 +746,7 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="G2" s="10"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -791,7 +783,7 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="11"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -828,7 +820,7 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -865,7 +857,7 @@
       <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -902,7 +894,7 @@
       <c r="F6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -939,7 +931,7 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -976,7 +968,7 @@
       <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1013,7 +1005,7 @@
       <c r="F9" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1050,7 +1042,7 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="11"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1087,7 +1079,7 @@
       <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="11"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1124,7 +1116,7 @@
       <c r="F12" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1161,7 +1153,7 @@
       <c r="F13" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1198,7 +1190,7 @@
       <c r="F14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1235,7 +1227,7 @@
       <c r="F15" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1272,7 +1264,7 @@
       <c r="F16" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <v>28239</v>
       </c>
       <c r="H16" s="1"/>
@@ -1311,7 +1303,7 @@
       <c r="F17" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1348,7 +1340,7 @@
       <c r="F18" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="10"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1385,7 +1377,7 @@
       <c r="F19" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="11"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1422,7 +1414,7 @@
       <c r="F20" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="11"/>
+      <c r="G20" s="10"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1459,7 +1451,7 @@
       <c r="F21" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="11"/>
+      <c r="G21" s="10"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1496,7 +1488,7 @@
       <c r="F22" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="11"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1533,7 +1525,7 @@
       <c r="F23" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="11"/>
+      <c r="G23" s="10"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1570,7 +1562,7 @@
       <c r="F24" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="11"/>
+      <c r="G24" s="10"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1607,7 +1599,7 @@
       <c r="F25" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="11"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1644,7 +1636,7 @@
       <c r="F26" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="11"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1681,7 +1673,7 @@
       <c r="F27" t="s">
         <v>7</v>
       </c>
-      <c r="G27" s="11"/>
+      <c r="G27" s="10"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1718,7 +1710,7 @@
       <c r="F28" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="11"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1755,7 +1747,7 @@
       <c r="F29" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="11"/>
+      <c r="G29" s="10"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1792,7 +1784,7 @@
       <c r="F30" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="11"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1829,7 +1821,7 @@
       <c r="F31" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="11"/>
+      <c r="G31" s="10"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1866,7 +1858,7 @@
       <c r="F32" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="11"/>
+      <c r="G32" s="10"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1903,7 +1895,7 @@
       <c r="F33" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="11"/>
+      <c r="G33" s="10"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1940,7 +1932,7 @@
       <c r="F34" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="11"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1977,7 +1969,7 @@
       <c r="F35" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="11"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2014,7 +2006,7 @@
       <c r="F36" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="11"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2051,7 +2043,7 @@
       <c r="F37" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="11"/>
+      <c r="G37" s="10"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -2088,7 +2080,7 @@
       <c r="F38" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="11"/>
+      <c r="G38" s="10"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2125,7 +2117,7 @@
       <c r="F39" t="s">
         <v>7</v>
       </c>
-      <c r="G39" s="11"/>
+      <c r="G39" s="10"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2162,7 +2154,7 @@
       <c r="F40" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="11"/>
+      <c r="G40" s="10"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2199,7 +2191,7 @@
       <c r="F41" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="11"/>
+      <c r="G41" s="10"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -2236,7 +2228,7 @@
       <c r="F42" t="s">
         <v>7</v>
       </c>
-      <c r="G42" s="11"/>
+      <c r="G42" s="10"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2273,7 +2265,7 @@
       <c r="F43" t="s">
         <v>13</v>
       </c>
-      <c r="G43" s="11"/>
+      <c r="G43" s="10"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2310,7 +2302,7 @@
       <c r="F44" t="s">
         <v>7</v>
       </c>
-      <c r="G44" s="11"/>
+      <c r="G44" s="10"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2347,7 +2339,7 @@
       <c r="F45" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="11"/>
+      <c r="G45" s="10"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2384,7 +2376,7 @@
       <c r="F46" t="s">
         <v>13</v>
       </c>
-      <c r="G46" s="11"/>
+      <c r="G46" s="10"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -2421,7 +2413,7 @@
       <c r="F47" t="s">
         <v>7</v>
       </c>
-      <c r="G47" s="11"/>
+      <c r="G47" s="10"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -2458,7 +2450,7 @@
       <c r="F48" t="s">
         <v>7</v>
       </c>
-      <c r="G48" s="11"/>
+      <c r="G48" s="10"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -2495,7 +2487,7 @@
       <c r="F49" t="s">
         <v>13</v>
       </c>
-      <c r="G49" s="11"/>
+      <c r="G49" s="10"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -2532,7 +2524,7 @@
       <c r="F50" t="s">
         <v>7</v>
       </c>
-      <c r="G50" s="11"/>
+      <c r="G50" s="10"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
@@ -2569,7 +2561,7 @@
       <c r="F51" t="s">
         <v>7</v>
       </c>
-      <c r="G51" s="11">
+      <c r="G51" s="10">
         <v>33562</v>
       </c>
       <c r="H51" s="1"/>
@@ -2608,7 +2600,7 @@
       <c r="F52" t="s">
         <v>13</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G52" s="10">
         <v>34480</v>
       </c>
       <c r="H52" s="1"/>
@@ -2647,7 +2639,7 @@
       <c r="F53" t="s">
         <v>7</v>
       </c>
-      <c r="G53" s="11">
+      <c r="G53" s="10">
         <v>36484</v>
       </c>
       <c r="H53" s="1"/>
@@ -2686,7 +2678,7 @@
       <c r="F54" t="s">
         <v>13</v>
       </c>
-      <c r="G54" s="11"/>
+      <c r="G54" s="10"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -2723,7 +2715,7 @@
       <c r="F55" t="s">
         <v>7</v>
       </c>
-      <c r="G55" s="11">
+      <c r="G55" s="10">
         <v>29258</v>
       </c>
       <c r="H55" s="1"/>
@@ -2762,7 +2754,7 @@
       <c r="F56" t="s">
         <v>7</v>
       </c>
-      <c r="G56" s="11"/>
+      <c r="G56" s="10"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -2799,7 +2791,7 @@
       <c r="F57" t="s">
         <v>13</v>
       </c>
-      <c r="G57" s="11"/>
+      <c r="G57" s="10"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -2836,7 +2828,7 @@
       <c r="F58" t="s">
         <v>7</v>
       </c>
-      <c r="G58" s="11"/>
+      <c r="G58" s="10"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -2873,7 +2865,7 @@
       <c r="F59" t="s">
         <v>7</v>
       </c>
-      <c r="G59" s="11">
+      <c r="G59" s="10">
         <v>36426</v>
       </c>
       <c r="H59" s="1"/>
@@ -2912,7 +2904,7 @@
       <c r="F60" t="s">
         <v>13</v>
       </c>
-      <c r="G60" s="11"/>
+      <c r="G60" s="10"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -2949,7 +2941,7 @@
       <c r="F61" t="s">
         <v>7</v>
       </c>
-      <c r="G61" s="11"/>
+      <c r="G61" s="10"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -2986,7 +2978,7 @@
       <c r="F62" t="s">
         <v>13</v>
       </c>
-      <c r="G62" s="11"/>
+      <c r="G62" s="10"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -3023,7 +3015,7 @@
       <c r="F63" t="s">
         <v>13</v>
       </c>
-      <c r="G63" s="11"/>
+      <c r="G63" s="10"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -3060,7 +3052,7 @@
       <c r="F64" t="s">
         <v>13</v>
       </c>
-      <c r="G64" s="11"/>
+      <c r="G64" s="10"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -3097,7 +3089,7 @@
       <c r="F65" t="s">
         <v>7</v>
       </c>
-      <c r="G65" s="11"/>
+      <c r="G65" s="10"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
@@ -3134,7 +3126,7 @@
       <c r="F66" t="s">
         <v>7</v>
       </c>
-      <c r="G66" s="11"/>
+      <c r="G66" s="10"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
@@ -3171,7 +3163,7 @@
       <c r="F67" t="s">
         <v>7</v>
       </c>
-      <c r="G67" s="11">
+      <c r="G67" s="10">
         <v>37602</v>
       </c>
       <c r="H67" s="1"/>
@@ -3210,7 +3202,7 @@
       <c r="F68" t="s">
         <v>7</v>
       </c>
-      <c r="G68" s="11">
+      <c r="G68" s="10">
         <v>39049</v>
       </c>
       <c r="H68" s="1"/>
@@ -3249,7 +3241,7 @@
       <c r="F69" t="s">
         <v>7</v>
       </c>
-      <c r="G69" s="11">
+      <c r="G69" s="10">
         <v>39877</v>
       </c>
       <c r="H69" s="1"/>
@@ -3288,7 +3280,7 @@
       <c r="F70" t="s">
         <v>13</v>
       </c>
-      <c r="G70" s="11">
+      <c r="G70" s="10">
         <v>40931</v>
       </c>
       <c r="H70" s="1"/>
@@ -3327,7 +3319,7 @@
       <c r="F71" t="s">
         <v>13</v>
       </c>
-      <c r="G71" s="11">
+      <c r="G71" s="10">
         <v>44379</v>
       </c>
       <c r="H71" s="1"/>
@@ -3366,7 +3358,7 @@
       <c r="F72" t="s">
         <v>7</v>
       </c>
-      <c r="G72" s="11"/>
+      <c r="G72" s="10"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
@@ -3403,7 +3395,7 @@
       <c r="F73" t="s">
         <v>7</v>
       </c>
-      <c r="G73" s="11"/>
+      <c r="G73" s="10"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -3440,7 +3432,7 @@
       <c r="F74" t="s">
         <v>7</v>
       </c>
-      <c r="G74" s="11"/>
+      <c r="G74" s="10"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
@@ -3477,7 +3469,7 @@
       <c r="F75" t="s">
         <v>13</v>
       </c>
-      <c r="G75" s="11"/>
+      <c r="G75" s="10"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
@@ -3514,7 +3506,7 @@
       <c r="F76" t="s">
         <v>13</v>
       </c>
-      <c r="G76" s="11"/>
+      <c r="G76" s="10"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -3551,7 +3543,7 @@
       <c r="F77" t="s">
         <v>7</v>
       </c>
-      <c r="G77" s="11"/>
+      <c r="G77" s="10"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
@@ -3588,7 +3580,7 @@
       <c r="F78" t="s">
         <v>7</v>
       </c>
-      <c r="G78" s="11"/>
+      <c r="G78" s="10"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
@@ -3625,7 +3617,7 @@
       <c r="F79" t="s">
         <v>13</v>
       </c>
-      <c r="G79" s="11"/>
+      <c r="G79" s="10"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
@@ -3662,7 +3654,7 @@
       <c r="F80" t="s">
         <v>7</v>
       </c>
-      <c r="G80" s="11"/>
+      <c r="G80" s="10"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
@@ -3699,7 +3691,7 @@
       <c r="F81" t="s">
         <v>13</v>
       </c>
-      <c r="G81" s="11"/>
+      <c r="G81" s="10"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -3736,7 +3728,7 @@
       <c r="F82" t="s">
         <v>7</v>
       </c>
-      <c r="G82" s="11"/>
+      <c r="G82" s="10"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -3773,7 +3765,7 @@
       <c r="F83" t="s">
         <v>13</v>
       </c>
-      <c r="G83" s="11"/>
+      <c r="G83" s="10"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -3810,7 +3802,7 @@
       <c r="F84" t="s">
         <v>13</v>
       </c>
-      <c r="G84" s="11">
+      <c r="G84" s="10">
         <v>45292</v>
       </c>
       <c r="H84" s="1"/>
@@ -3849,7 +3841,7 @@
       <c r="F85" t="s">
         <v>7</v>
       </c>
-      <c r="G85" s="11">
+      <c r="G85" s="10">
         <v>44214</v>
       </c>
       <c r="H85" s="1"/>
@@ -3888,7 +3880,7 @@
       <c r="F86" t="s">
         <v>7</v>
       </c>
-      <c r="G86" s="11"/>
+      <c r="G86" s="10"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
@@ -3925,7 +3917,7 @@
       <c r="F87" t="s">
         <v>7</v>
       </c>
-      <c r="G87" s="11">
+      <c r="G87" s="10">
         <v>44214</v>
       </c>
       <c r="H87" s="1"/>
@@ -3964,7 +3956,7 @@
       <c r="F88" t="s">
         <v>13</v>
       </c>
-      <c r="G88" s="11"/>
+      <c r="G88" s="10"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
@@ -4001,7 +3993,7 @@
       <c r="F89" t="s">
         <v>13</v>
       </c>
-      <c r="G89" s="11"/>
+      <c r="G89" s="10"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
@@ -4038,7 +4030,7 @@
       <c r="F90" t="s">
         <v>13</v>
       </c>
-      <c r="G90" s="11"/>
+      <c r="G90" s="10"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>

</xml_diff>

<commit_message>
Updated for Kulsoom Zahra (04-21-2024)
</commit_message>
<xml_diff>
--- a/public/resources/data/JanAliFamilyDatabase.xlsx
+++ b/public/resources/data/JanAliFamilyDatabase.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JanAli\janalisinformation\frontend\janaliinformationsystem\public\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F16611-4DAD-4E91-85C9-4FFFC292F182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DD0563-159D-43D3-AEFE-89F7D24A2EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="124">
   <si>
     <t>Id</t>
   </si>
@@ -370,6 +371,30 @@
   <si>
     <t>Hania Batool</t>
   </si>
+  <si>
+    <t>Kulsoom Zahra</t>
+  </si>
+  <si>
+    <t>Zahida Batool</t>
+  </si>
+  <si>
+    <t>Qasim</t>
+  </si>
+  <si>
+    <t>Jahan Zaib</t>
+  </si>
+  <si>
+    <t>Ghulam Ali</t>
+  </si>
+  <si>
+    <t>Ali Yar</t>
+  </si>
+  <si>
+    <t>Jahan Baig</t>
+  </si>
+  <si>
+    <t>Ghoto</t>
+  </si>
 </sst>
 </file>
 
@@ -451,7 +476,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,8 +579,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -622,11 +653,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -754,6 +805,39 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -26169,10 +26253,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EE6260-2E3B-473B-9EDE-07426FA9F207}">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="92" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView topLeftCell="A86" zoomScale="92" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26647,11 +26731,11 @@
       </c>
       <c r="H16" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>46 years, 10 months</v>
+        <v>46 years, 11 months</v>
       </c>
       <c r="I16" s="47" t="str">
         <f ca="1">IF(G16="", "", IF(DATE(YEAR(TODAY()),MONTH(G16),DAY(G16))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G16),DAY(G16))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G16),DAY(G16))-TODAY()) &amp; " Days" )</f>
-        <v>52 Days</v>
+        <v>3 Days</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -27577,11 +27661,11 @@
       </c>
       <c r="H48" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>44 years, 0 months</v>
+        <v>44 years, 2 months</v>
       </c>
       <c r="I48" s="47" t="str">
         <f ca="1">IF(G48="", "", IF(DATE(YEAR(TODAY()),MONTH(G48),DAY(G48))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G48),DAY(G48))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G48),DAY(G48))-TODAY()) &amp; " Days" )</f>
-        <v>341 Days</v>
+        <v>292 Days</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -27666,11 +27750,11 @@
       </c>
       <c r="H51" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>32 years, 3 months</v>
+        <v>32 years, 5 months</v>
       </c>
       <c r="I51" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>262 Days</v>
+        <v>213 Days</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -27697,11 +27781,11 @@
       </c>
       <c r="H52" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>29 years, 9 months</v>
+        <v>29 years, 10 months</v>
       </c>
       <c r="I52" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>84 Days</v>
+        <v>35 Days</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -27728,11 +27812,11 @@
       </c>
       <c r="H53" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24 years, 3 months</v>
+        <v>24 years, 5 months</v>
       </c>
       <c r="I53" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>262 Days</v>
+        <v>213 Days</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -27846,11 +27930,11 @@
       </c>
       <c r="H57" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>29 years, 8 months</v>
+        <v>29 years, 9 months</v>
       </c>
       <c r="I57" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>115 Days</v>
+        <v>66 Days</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -27877,11 +27961,11 @@
       </c>
       <c r="H58" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26 years, 3 months</v>
+        <v>26 years, 5 months</v>
       </c>
       <c r="I58" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>252 Days</v>
+        <v>203 Days</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -27908,11 +27992,11 @@
       </c>
       <c r="H59" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24 years, 5 months</v>
+        <v>24 years, 6 months</v>
       </c>
       <c r="I59" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>204 Days</v>
+        <v>155 Days</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -27997,11 +28081,11 @@
       </c>
       <c r="H62" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22 years, 11 months</v>
+        <v>23 years, 1 months</v>
       </c>
       <c r="I62" s="47" t="str">
         <f ca="1">IF(G62="", "", IF(DATE(YEAR(TODAY()),MONTH(G62),DAY(G62))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G62),DAY(G62))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G62),DAY(G62))-TODAY()) &amp; " Days" )</f>
-        <v>15 Days</v>
+        <v>331 Days</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28028,11 +28112,11 @@
       </c>
       <c r="H63" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20 years, 8 months</v>
+        <v>20 years, 10 months</v>
       </c>
       <c r="I63" s="47" t="str">
         <f ca="1">IF(G63="", "", IF(DATE(YEAR(TODAY()),MONTH(G63),DAY(G63))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G63),DAY(G63))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G63),DAY(G63))-TODAY()) &amp; " Days" )</f>
-        <v>102 Days</v>
+        <v>53 Days</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28059,11 +28143,11 @@
       </c>
       <c r="H64" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17 years, 3 months</v>
+        <v>17 years, 4 months</v>
       </c>
       <c r="I64" s="47" t="str">
         <f t="shared" ref="I64:I91" ca="1" si="4">IF(G64="", "", IF(DATE(YEAR(TODAY()),MONTH(G64),DAY(G64))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G64),DAY(G64))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G64),DAY(G64))-TODAY()) &amp; " Days" )</f>
-        <v>264 Days</v>
+        <v>215 Days</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28090,11 +28174,11 @@
       </c>
       <c r="H65" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14 years, 2 months</v>
+        <v>14 years, 4 months</v>
       </c>
       <c r="I65" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>287 Days</v>
+        <v>238 Days</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28121,11 +28205,11 @@
       </c>
       <c r="H66" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7 years, 3 months</v>
+        <v>7 years, 5 months</v>
       </c>
       <c r="I66" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>246 Days</v>
+        <v>197 Days</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28152,11 +28236,11 @@
       </c>
       <c r="H67" s="16" t="str">
         <f t="shared" ref="H67:H91" ca="1" si="5">IF(G67="", "", DATEDIF(G67, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G67, TODAY(), "YM") &amp; " months")</f>
-        <v>21 years, 2 months</v>
+        <v>21 years, 4 months</v>
       </c>
       <c r="I67" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>284 Days</v>
+        <v>235 Days</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28183,11 +28267,11 @@
       </c>
       <c r="H68" s="16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>17 years, 3 months</v>
+        <v>17 years, 4 months</v>
       </c>
       <c r="I68" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>270 Days</v>
+        <v>221 Days</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28214,11 +28298,11 @@
       </c>
       <c r="H69" s="16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>14 years, 11 months</v>
+        <v>15 years, 1 months</v>
       </c>
       <c r="I69" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>2 Days</v>
+        <v>318 Days</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28245,11 +28329,11 @@
       </c>
       <c r="H70" s="16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>12 years, 1 months</v>
+        <v>12 years, 2 months</v>
       </c>
       <c r="I70" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>326 Days</v>
+        <v>277 Days</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28276,11 +28360,11 @@
       </c>
       <c r="H71" s="16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>2 years, 8 months</v>
+        <v>2 years, 9 months</v>
       </c>
       <c r="I71" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>121 Days</v>
+        <v>72 Days</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28655,11 +28739,11 @@
       </c>
       <c r="H84" s="16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0 years, 2 months</v>
+        <v>0 years, 3 months</v>
       </c>
       <c r="I84" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>304 Days</v>
+        <v>255 Days</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28686,11 +28770,11 @@
       </c>
       <c r="H85" s="16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>3 years, 1 months</v>
+        <v>3 years, 3 months</v>
       </c>
       <c r="I85" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>321 Days</v>
+        <v>272 Days</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28746,11 +28830,11 @@
       </c>
       <c r="H87" s="16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>4 years, 1 months</v>
+        <v>4 years, 3 months</v>
       </c>
       <c r="I87" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>321 Days</v>
+        <v>272 Days</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28869,7 +28953,3015 @@
         <v/>
       </c>
     </row>
+    <row r="92" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>58</v>
+      </c>
+      <c r="C92" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="D92" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="E92" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="F92" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" s="48">
+        <v>45394</v>
+      </c>
+      <c r="H92" s="16" t="str">
+        <f t="shared" ref="H92" ca="1" si="6">IF(G92="", "", DATEDIF(G92, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G92, TODAY(), "YM") &amp; " months")</f>
+        <v>0 years, 0 months</v>
+      </c>
+      <c r="I92" s="47" t="str">
+        <f t="shared" ref="I92" ca="1" si="7">IF(G92="", "", IF(DATE(YEAR(TODAY()),MONTH(G92),DAY(G92))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G92),DAY(G92))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G92),DAY(G92))-TODAY()) &amp; " Days" )</f>
+        <v>356 Days</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF14398D-78BE-4B6D-AD2F-2626D9C6A9FD}">
+  <dimension ref="A1:I108"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="52"/>
+    </row>
+    <row r="3" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="52"/>
+    </row>
+    <row r="4" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="52"/>
+    </row>
+    <row r="5" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16" t="str">
+        <f ca="1">IF(G5="", "", DATEDIF(G5, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G5, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I5" s="47" t="str">
+        <f ca="1">IF(G5="", "", IF(DATE(YEAR(TODAY()),MONTH(G5),DAY(G5))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G5),DAY(G5))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G5),DAY(G5))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16" t="str">
+        <f t="shared" ref="H6:H9" ca="1" si="0">IF(G6="", "", DATEDIF(G6, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G6, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I6" s="47" t="str">
+        <f ca="1">IF(G6="", "", IF(DATE(YEAR(TODAY()),MONTH(G6),DAY(G6))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G6),DAY(G6))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G6),DAY(G6))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="I7" s="47" t="str">
+        <f t="shared" ref="I7:I9" ca="1" si="1">IF(G7="", "", IF(DATE(YEAR(TODAY()),MONTH(G7),DAY(G7))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G7),DAY(G7))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G7),DAY(G7))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="I8" s="47" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="I9" s="47" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16" t="str">
+        <f ca="1">IF(G10="", "", DATEDIF(G10, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G10, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I10" s="47" t="str">
+        <f ca="1">IF(G10="", "", IF(DATE(YEAR(TODAY()),MONTH(G10),DAY(G10))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G10),DAY(G10))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G10),DAY(G10))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16" t="str">
+        <f t="shared" ref="H11:H74" ca="1" si="2">IF(G11="", "", DATEDIF(G11, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G11, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I11" s="47" t="str">
+        <f ca="1">IF(G11="", "", IF(DATE(YEAR(TODAY()),MONTH(G11),DAY(G11))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G11),DAY(G11))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G11),DAY(G11))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16" t="str">
+        <f t="shared" ref="H12:H75" ca="1" si="3">IF(G12="", "", DATEDIF(G12, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G12, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I12" s="47" t="str">
+        <f t="shared" ref="I12:I34" ca="1" si="4">IF(G12="", "", IF(DATE(YEAR(TODAY()),MONTH(G12),DAY(G12))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G12),DAY(G12))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G12),DAY(G12))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16" t="str">
+        <f t="shared" ref="H13:H76" ca="1" si="5">IF(G13="", "", DATEDIF(G13, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G13, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I13" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16" t="str">
+        <f t="shared" ref="H14:H77" ca="1" si="6">IF(G14="", "", DATEDIF(G14, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G14, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I14" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16" t="str">
+        <f t="shared" ref="H15:H78" ca="1" si="7">IF(G15="", "", DATEDIF(G15, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G15, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I15" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="str">
+        <f t="shared" ref="H16:H79" ca="1" si="8">IF(G16="", "", DATEDIF(G16, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G16, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I16" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16" t="str">
+        <f t="shared" ref="H17:H80" ca="1" si="9">IF(G17="", "", DATEDIF(G17, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G17, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I17" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16" t="str">
+        <f t="shared" ref="H18:H81" ca="1" si="10">IF(G18="", "", DATEDIF(G18, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G18, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I18" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16" t="str">
+        <f t="shared" ref="H19:H82" ca="1" si="11">IF(G19="", "", DATEDIF(G19, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G19, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I19" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>11</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16" t="str">
+        <f t="shared" ref="H20:H83" ca="1" si="12">IF(G20="", "", DATEDIF(G20, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G20, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I20" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>11</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16" t="str">
+        <f t="shared" ref="H21:H84" ca="1" si="13">IF(G21="", "", DATEDIF(G21, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G21, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I21" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16" t="str">
+        <f t="shared" ref="H22:H85" ca="1" si="14">IF(G22="", "", DATEDIF(G22, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G22, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I22" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>11</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16" t="str">
+        <f t="shared" ref="H23:H86" ca="1" si="15">IF(G23="", "", DATEDIF(G23, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G23, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I23" s="47" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="17">
+        <v>28239</v>
+      </c>
+      <c r="H24" s="16" t="str">
+        <f t="shared" ref="H24:H87" ca="1" si="16">IF(G24="", "", DATEDIF(G24, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G24, TODAY(), "YM") &amp; " months")</f>
+        <v>46 years, 11 months</v>
+      </c>
+      <c r="I24" s="47" t="str">
+        <f ca="1">IF(G24="", "", IF(DATE(YEAR(TODAY()),MONTH(G24),DAY(G24))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G24),DAY(G24))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G24),DAY(G24))-TODAY()) &amp; " Days" )</f>
+        <v>3 Days</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>11</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16" t="str">
+        <f t="shared" ref="H25:H88" ca="1" si="17">IF(G25="", "", DATEDIF(G25, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G25, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I25" s="47" t="str">
+        <f ca="1">IF(G25="", "", IF(DATE(YEAR(TODAY()),MONTH(G25),DAY(G25))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G25),DAY(G25))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G25),DAY(G25))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>11</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16" t="str">
+        <f t="shared" ref="H26:H89" ca="1" si="18">IF(G26="", "", DATEDIF(G26, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G26, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I26" s="47" t="str">
+        <f t="shared" ref="I26:I84" ca="1" si="19">IF(G26="", "", IF(DATE(YEAR(TODAY()),MONTH(G26),DAY(G26))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G26),DAY(G26))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G26),DAY(G26))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>11</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16" t="str">
+        <f t="shared" ref="H27:H90" ca="1" si="20">IF(G27="", "", DATEDIF(G27, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G27, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I27" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>11</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16" t="str">
+        <f t="shared" ref="H28:H91" ca="1" si="21">IF(G28="", "", DATEDIF(G28, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G28, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I28" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>12</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16" t="str">
+        <f t="shared" ref="H29:H92" ca="1" si="22">IF(G29="", "", DATEDIF(G29, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G29, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I29" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16" t="str">
+        <f t="shared" ref="H30:H93" ca="1" si="23">IF(G30="", "", DATEDIF(G30, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G30, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I30" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16" t="str">
+        <f t="shared" ref="H31:H94" ca="1" si="24">IF(G31="", "", DATEDIF(G31, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G31, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I31" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16" t="str">
+        <f t="shared" ref="H32:H95" ca="1" si="25">IF(G32="", "", DATEDIF(G32, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G32, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I32" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>13</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16" t="str">
+        <f t="shared" ref="H33:H96" ca="1" si="26">IF(G33="", "", DATEDIF(G33, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G33, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I33" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>13</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16" t="str">
+        <f t="shared" ref="H34:H97" ca="1" si="27">IF(G34="", "", DATEDIF(G34, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G34, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I34" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>13</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16" t="str">
+        <f t="shared" ref="H35:H98" ca="1" si="28">IF(G35="", "", DATEDIF(G35, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G35, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I35" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>13</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16" t="str">
+        <f t="shared" ref="H36:H99" ca="1" si="29">IF(G36="", "", DATEDIF(G36, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G36, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I36" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>13</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16" t="str">
+        <f t="shared" ref="H37:H100" ca="1" si="30">IF(G37="", "", DATEDIF(G37, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G37, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I37" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>13</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I38" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>14</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I39" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I40" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>14</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I41" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>14</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I42" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>14</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I43" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>14</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I44" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>14</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I45" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>14</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I46" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>15</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F47" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I47" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>15</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I48" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I49" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>15</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I50" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>15</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I51" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>16</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I52" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>16</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I53" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>16</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F54" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I54" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>16</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I55" s="47" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>19</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="17">
+        <v>29258</v>
+      </c>
+      <c r="H56" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>44 years, 2 months</v>
+      </c>
+      <c r="I56" s="47" t="str">
+        <f ca="1">IF(G56="", "", IF(DATE(YEAR(TODAY()),MONTH(G56),DAY(G56))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G56),DAY(G56))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G56),DAY(G56))-TODAY()) &amp; " Days" )</f>
+        <v>292 Days</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>19</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I57" s="47" t="str">
+        <f ca="1">IF(G57="", "", IF(DATE(YEAR(TODAY()),MONTH(G57),DAY(G57))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G57),DAY(G57))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G57),DAY(G57))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>19</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I58" s="47" t="str">
+        <f t="shared" ref="I58:I80" ca="1" si="31">IF(G58="", "", IF(DATE(YEAR(TODAY()),MONTH(G58),DAY(G58))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G58),DAY(G58))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G58),DAY(G58))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>19</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="17">
+        <v>33562</v>
+      </c>
+      <c r="H59" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>32 years, 5 months</v>
+      </c>
+      <c r="I59" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>213 Days</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>19</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="17">
+        <v>34480</v>
+      </c>
+      <c r="H60" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>29 years, 10 months</v>
+      </c>
+      <c r="I60" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>35 Days</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>19</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="17">
+        <v>36484</v>
+      </c>
+      <c r="H61" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>24 years, 5 months</v>
+      </c>
+      <c r="I61" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>213 Days</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>19</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I62" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>20</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I63" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>20</v>
+      </c>
+      <c r="C64" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I64" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>20</v>
+      </c>
+      <c r="C65" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F65" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="17">
+        <v>34511</v>
+      </c>
+      <c r="H65" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>29 years, 9 months</v>
+      </c>
+      <c r="I65" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>66 Days</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>20</v>
+      </c>
+      <c r="C66" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F66" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" s="17">
+        <v>35744</v>
+      </c>
+      <c r="H66" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>26 years, 5 months</v>
+      </c>
+      <c r="I66" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>203 Days</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>20</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G67" s="17">
+        <v>36426</v>
+      </c>
+      <c r="H67" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>24 years, 6 months</v>
+      </c>
+      <c r="I67" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>155 Days</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>20</v>
+      </c>
+      <c r="C68" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F68" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I68" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>20</v>
+      </c>
+      <c r="C69" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F69" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I69" s="47" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>22</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" s="17">
+        <v>36968</v>
+      </c>
+      <c r="H70" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>23 years, 1 months</v>
+      </c>
+      <c r="I70" s="47" t="str">
+        <f ca="1">IF(G70="", "", IF(DATE(YEAR(TODAY()),MONTH(G70),DAY(G70))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G70),DAY(G70))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G70),DAY(G70))-TODAY()) &amp; " Days" )</f>
+        <v>331 Days</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>22</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G71" s="17">
+        <v>37785</v>
+      </c>
+      <c r="H71" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>20 years, 10 months</v>
+      </c>
+      <c r="I71" s="47" t="str">
+        <f ca="1">IF(G71="", "", IF(DATE(YEAR(TODAY()),MONTH(G71),DAY(G71))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G71),DAY(G71))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G71),DAY(G71))-TODAY()) &amp; " Days" )</f>
+        <v>53 Days</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>22</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D72" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="17">
+        <v>39043</v>
+      </c>
+      <c r="H72" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>17 years, 4 months</v>
+      </c>
+      <c r="I72" s="47" t="str">
+        <f t="shared" ref="I72:I100" ca="1" si="32">IF(G72="", "", IF(DATE(YEAR(TODAY()),MONTH(G72),DAY(G72))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G72),DAY(G72))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G72),DAY(G72))-TODAY()) &amp; " Days" )</f>
+        <v>215 Days</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>22</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E73" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F73" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" s="17">
+        <v>40162</v>
+      </c>
+      <c r="H73" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>14 years, 4 months</v>
+      </c>
+      <c r="I73" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>238 Days</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>22</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D74" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F74" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" s="17">
+        <v>42678</v>
+      </c>
+      <c r="H74" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>7 years, 5 months</v>
+      </c>
+      <c r="I74" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>197 Days</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>23</v>
+      </c>
+      <c r="C75" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D75" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F75" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" s="17">
+        <v>37602</v>
+      </c>
+      <c r="H75" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>21 years, 4 months</v>
+      </c>
+      <c r="I75" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>235 Days</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>23</v>
+      </c>
+      <c r="C76" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F76" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76" s="17">
+        <v>39049</v>
+      </c>
+      <c r="H76" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>17 years, 4 months</v>
+      </c>
+      <c r="I76" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>221 Days</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>23</v>
+      </c>
+      <c r="C77" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D77" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F77" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77" s="17">
+        <v>39877</v>
+      </c>
+      <c r="H77" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>15 years, 1 months</v>
+      </c>
+      <c r="I77" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>318 Days</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>23</v>
+      </c>
+      <c r="C78" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D78" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F78" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G78" s="17">
+        <v>40931</v>
+      </c>
+      <c r="H78" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>12 years, 2 months</v>
+      </c>
+      <c r="I78" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>277 Days</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>23</v>
+      </c>
+      <c r="C79" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D79" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="17">
+        <v>44379</v>
+      </c>
+      <c r="H79" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>2 years, 9 months</v>
+      </c>
+      <c r="I79" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>72 Days</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>27</v>
+      </c>
+      <c r="C80" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D80" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E80" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F80" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I80" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>27</v>
+      </c>
+      <c r="C81" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D81" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E81" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F81" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I81" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>55</v>
+      </c>
+      <c r="C82" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D82" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E82" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F82" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I82" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>55</v>
+      </c>
+      <c r="C83" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D83" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E83" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F83" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G83" s="16"/>
+      <c r="H83" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I83" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>55</v>
+      </c>
+      <c r="C84" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D84" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E84" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F84" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I84" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>55</v>
+      </c>
+      <c r="C85" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D85" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E85" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F85" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I85" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>55</v>
+      </c>
+      <c r="C86" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D86" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E86" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F86" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G86" s="16"/>
+      <c r="H86" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I86" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>57</v>
+      </c>
+      <c r="C87" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D87" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="E87" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F87" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G87" s="16"/>
+      <c r="H87" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I87" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>57</v>
+      </c>
+      <c r="C88" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D88" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="E88" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F88" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G88" s="16"/>
+      <c r="H88" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I88" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>57</v>
+      </c>
+      <c r="C89" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D89" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="E89" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F89" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G89" s="16"/>
+      <c r="H89" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I89" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>57</v>
+      </c>
+      <c r="C90" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D90" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="E90" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F90" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G90" s="16"/>
+      <c r="H90" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I90" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>58</v>
+      </c>
+      <c r="C91" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D91" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E91" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G91" s="16"/>
+      <c r="H91" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I91" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>58</v>
+      </c>
+      <c r="C92" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D92" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" s="17">
+        <v>45292</v>
+      </c>
+      <c r="H92" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>0 years, 3 months</v>
+      </c>
+      <c r="I92" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>255 Days</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>62</v>
+      </c>
+      <c r="C93" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="D93" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E93" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F93" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G93" s="17">
+        <v>44214</v>
+      </c>
+      <c r="H93" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>3 years, 3 months</v>
+      </c>
+      <c r="I93" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>272 Days</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>63</v>
+      </c>
+      <c r="C94" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E94" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F94" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G94" s="16"/>
+      <c r="H94" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I94" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>63</v>
+      </c>
+      <c r="C95" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D95" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E95" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F95" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G95" s="17">
+        <v>43848</v>
+      </c>
+      <c r="H95" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>4 years, 3 months</v>
+      </c>
+      <c r="I95" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>272 Days</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>46</v>
+      </c>
+      <c r="C96" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D96" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E96" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="F96" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G96" s="16"/>
+      <c r="H96" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I96" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>46</v>
+      </c>
+      <c r="C97" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D97" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E97" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="F97" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G97" s="16"/>
+      <c r="H97" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I97" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>49</v>
+      </c>
+      <c r="C98" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D98" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="E98" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="F98" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I98" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>42</v>
+      </c>
+      <c r="C99" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D99" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E99" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="F99" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="16"/>
+      <c r="H99" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="I99" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>66</v>
+      </c>
+      <c r="C100" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="D100" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="E100" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="F100" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" s="17">
+        <v>45394</v>
+      </c>
+      <c r="H100" s="16" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v>0 years, 0 months</v>
+      </c>
+      <c r="I100" s="47" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>356 Days</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G101"/>
+    </row>
+    <row r="102" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G102"/>
+    </row>
+    <row r="103" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G103"/>
+    </row>
+    <row r="104" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G104"/>
+    </row>
+    <row r="105" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G105"/>
+    </row>
+    <row r="106" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G106"/>
+    </row>
+    <row r="107" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G107"/>
+    </row>
+    <row r="108" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G108"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data translated to urdu.
</commit_message>
<xml_diff>
--- a/public/resources/data/JanAliFamilyDatabase.xlsx
+++ b/public/resources/data/JanAliFamilyDatabase.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Side\JanAli\familytree\janaliinformationsystem\public\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4A35BF-5A9A-4D5A-862B-AD75B8096711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC88415-7100-4D6C-9212-B0FCA7A2714A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="EnglishSheet" sheetId="2" r:id="rId1"/>
+    <sheet name="UrduSheet" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="221">
   <si>
     <t>Id</t>
   </si>
@@ -381,24 +381,6 @@
     <t>Zahida Batool</t>
   </si>
   <si>
-    <t>Qasim</t>
-  </si>
-  <si>
-    <t>Jahan Zaib</t>
-  </si>
-  <si>
-    <t>Ghulam Ali</t>
-  </si>
-  <si>
-    <t>Ali Yar</t>
-  </si>
-  <si>
-    <t>Jahan Baig</t>
-  </si>
-  <si>
-    <t>Ghoto</t>
-  </si>
-  <si>
     <t>Dua Narjis</t>
   </si>
   <si>
@@ -406,6 +388,315 @@
   </si>
   <si>
     <t>Rahman Ali</t>
+  </si>
+  <si>
+    <t>جان علی</t>
+  </si>
+  <si>
+    <t>حسین</t>
+  </si>
+  <si>
+    <t>محمد علی</t>
+  </si>
+  <si>
+    <t>عبدالرحمن</t>
+  </si>
+  <si>
+    <t>حسن علی</t>
+  </si>
+  <si>
+    <t>اشچو فاطمہ</t>
+  </si>
+  <si>
+    <t>محمد جان</t>
+  </si>
+  <si>
+    <t>محمد رضا</t>
+  </si>
+  <si>
+    <t>اصغر علی</t>
+  </si>
+  <si>
+    <t>حسن جان</t>
+  </si>
+  <si>
+    <t>رقیہ بتول</t>
+  </si>
+  <si>
+    <t>صغرا فاطمہ</t>
+  </si>
+  <si>
+    <t>محمد تقی</t>
+  </si>
+  <si>
+    <t>کلثوم بی بی</t>
+  </si>
+  <si>
+    <t>محمد صادق</t>
+  </si>
+  <si>
+    <t>حاجرہ بتول</t>
+  </si>
+  <si>
+    <t>محمد یوسف</t>
+  </si>
+  <si>
+    <t>محمد ایوب</t>
+  </si>
+  <si>
+    <t>خیر النساء</t>
+  </si>
+  <si>
+    <t>زینب بی</t>
+  </si>
+  <si>
+    <t>نرگس خاتون</t>
+  </si>
+  <si>
+    <t>حبیب اللہ</t>
+  </si>
+  <si>
+    <t>غلام حیدر</t>
+  </si>
+  <si>
+    <t>نرگس بتول</t>
+  </si>
+  <si>
+    <t>منیر</t>
+  </si>
+  <si>
+    <t>زیبا</t>
+  </si>
+  <si>
+    <t>سکینہ</t>
+  </si>
+  <si>
+    <t>ساجدہ بتول</t>
+  </si>
+  <si>
+    <t>زہرا</t>
+  </si>
+  <si>
+    <t>کنیز فاطمہ</t>
+  </si>
+  <si>
+    <t>انیس فاطمہ</t>
+  </si>
+  <si>
+    <t>سعدیہ</t>
+  </si>
+  <si>
+    <t>محمد عقیل</t>
+  </si>
+  <si>
+    <t>بتول</t>
+  </si>
+  <si>
+    <t>صدیقہ بتول</t>
+  </si>
+  <si>
+    <t>محمد اسماعیل</t>
+  </si>
+  <si>
+    <t>محمد ظہیر</t>
+  </si>
+  <si>
+    <t>شبانہ بتول</t>
+  </si>
+  <si>
+    <t>امینہ بتول</t>
+  </si>
+  <si>
+    <t>غلام محمد</t>
+  </si>
+  <si>
+    <t>محمد افتخار</t>
+  </si>
+  <si>
+    <t>فاطمہ</t>
+  </si>
+  <si>
+    <t>خدیجہ</t>
+  </si>
+  <si>
+    <t>حکیمہ</t>
+  </si>
+  <si>
+    <t>باسط علی</t>
+  </si>
+  <si>
+    <t>حسیں</t>
+  </si>
+  <si>
+    <t>محمد یاسر</t>
+  </si>
+  <si>
+    <t>رحیمہ بتول</t>
+  </si>
+  <si>
+    <t>محمد ناصر</t>
+  </si>
+  <si>
+    <t>عروج زہرا</t>
+  </si>
+  <si>
+    <t>اشرف حسین</t>
+  </si>
+  <si>
+    <t>زیب النساء</t>
+  </si>
+  <si>
+    <t>غلام عباس</t>
+  </si>
+  <si>
+    <t>وجاہت حسین</t>
+  </si>
+  <si>
+    <t>محمد اکبر</t>
+  </si>
+  <si>
+    <t>محمد حسین</t>
+  </si>
+  <si>
+    <t>ناصرہ بتول</t>
+  </si>
+  <si>
+    <t>کمال علی اکمل</t>
+  </si>
+  <si>
+    <t>رضیہ فاطمہ</t>
+  </si>
+  <si>
+    <t>رحیمہ بی بی</t>
+  </si>
+  <si>
+    <t>سیرت فاطمہ</t>
+  </si>
+  <si>
+    <t>محمد عون</t>
+  </si>
+  <si>
+    <t>محمد زین حیدر</t>
+  </si>
+  <si>
+    <t>محمد یاور</t>
+  </si>
+  <si>
+    <t>جواد علی</t>
+  </si>
+  <si>
+    <t>محب علی</t>
+  </si>
+  <si>
+    <t>محدثہ فاطمہ</t>
+  </si>
+  <si>
+    <t>شجاع حیدر</t>
+  </si>
+  <si>
+    <t>کامل علی</t>
+  </si>
+  <si>
+    <t>ریحان اشرف</t>
+  </si>
+  <si>
+    <t>رضیہ بتول</t>
+  </si>
+  <si>
+    <t>روبینہ بتول</t>
+  </si>
+  <si>
+    <t>حجاب زہرا</t>
+  </si>
+  <si>
+    <t>جرّار حیدر</t>
+  </si>
+  <si>
+    <t>نرجس فاطمہ</t>
+  </si>
+  <si>
+    <t>نائمہ بتول</t>
+  </si>
+  <si>
+    <t>مظہر عباس</t>
+  </si>
+  <si>
+    <t>انعم بتول</t>
+  </si>
+  <si>
+    <t>میثم عباس</t>
+  </si>
+  <si>
+    <t>ہانیہ زہرا</t>
+  </si>
+  <si>
+    <t>ہادیہ زہرا</t>
+  </si>
+  <si>
+    <t>محسن حیدر</t>
+  </si>
+  <si>
+    <t>محمد نقی</t>
+  </si>
+  <si>
+    <t>رحمان علی</t>
+  </si>
+  <si>
+    <t>انسیہ مریم</t>
+  </si>
+  <si>
+    <t>نجمہ بتول</t>
+  </si>
+  <si>
+    <t>دیا زہرا</t>
+  </si>
+  <si>
+    <t>ولیہ زینب</t>
+  </si>
+  <si>
+    <t>حاجرہ</t>
+  </si>
+  <si>
+    <t>ہانیہ بتول</t>
+  </si>
+  <si>
+    <t>شاہدہ بتول</t>
+  </si>
+  <si>
+    <t>کلثوم زہرا</t>
+  </si>
+  <si>
+    <t>زاہدہ بتول</t>
+  </si>
+  <si>
+    <t>دعا نرجس</t>
+  </si>
+  <si>
+    <t>سائمہ بتول</t>
+  </si>
+  <si>
+    <t>ارج کلثوم</t>
+  </si>
+  <si>
+    <t>مظاہر حسین</t>
+  </si>
+  <si>
+    <t>کمیل علی</t>
+  </si>
+  <si>
+    <t>ثقلین مشتاق</t>
+  </si>
+  <si>
+    <t>خیزران فاطمہ</t>
+  </si>
+  <si>
+    <t>رجا فاطمہ</t>
+  </si>
+  <si>
+    <t>ردا فاطمہ</t>
+  </si>
+  <si>
+    <t>کرار حیدر</t>
   </si>
 </sst>
 </file>
@@ -413,7 +704,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -641,22 +932,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="4" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -746,7 +1037,7 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -754,30 +1045,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EE6260-2E3B-473B-9EDE-07426FA9F207}">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="92" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.54296875" defaultRowHeight="19.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1280,7 @@
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3586,7 +3853,7 @@
         <v>55</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D88" s="21" t="s">
         <v>63</v>
@@ -3764,13 +4031,13 @@
         <v>57</v>
       </c>
       <c r="C94" s="37" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D94" s="37" t="s">
         <v>65</v>
       </c>
       <c r="E94" s="37" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F94" s="38" t="s">
         <v>13</v>
@@ -3793,11 +4060,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF14398D-78BE-4B6D-AD2F-2626D9C6A9FD}">
-  <dimension ref="A1:I108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504FAD6C-E9C3-4525-B62C-93AAA300E3AA}">
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" zoomScale="92" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView topLeftCell="A6" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.54296875" defaultRowHeight="19.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3813,7 +4080,7 @@
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3842,7 +4109,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3850,22 +4117,28 @@
         <v>0</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="40"/>
-    </row>
-    <row r="3" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="str">
+        <f ca="1">IF(G2="", "", DATEDIF(G2, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G2, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I2" s="35" t="str">
+        <f ca="1">IF(G2="", "", IF(DATE(YEAR(TODAY()),MONTH(G2),DAY(G2))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G2),DAY(G2))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G2),DAY(G2))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3873,43 +4146,55 @@
         <v>1</v>
       </c>
       <c r="C3" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="31" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="40"/>
+      <c r="H3" s="4" t="str">
+        <f t="shared" ref="H3:H66" ca="1" si="0">IF(G3="", "", DATEDIF(G3, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G3, TODAY(), "YM") &amp; " months")</f>
+        <v/>
+      </c>
+      <c r="I3" s="35" t="str">
+        <f ca="1">IF(G3="", "", IF(DATE(YEAR(TODAY()),MONTH(G3),DAY(G3))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G3),DAY(G3))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G3),DAY(G3))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="31" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="40"/>
+      <c r="H4" s="4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="I4" s="35" t="str">
+        <f t="shared" ref="I4:I15" ca="1" si="1">IF(G4="", "", IF(DATE(YEAR(TODAY()),MONTH(G4),DAY(G4))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G4),DAY(G4))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G4),DAY(G4))-TODAY()) &amp; " Days" )</f>
+        <v/>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -3918,25 +4203,25 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="45" t="s">
+      <c r="C5" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="str">
-        <f ca="1">IF(G5="", "", DATEDIF(G5, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G5, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I5" s="35" t="str">
-        <f ca="1">IF(G5="", "", IF(DATE(YEAR(TODAY()),MONTH(G5),DAY(G5))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G5),DAY(G5))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G5),DAY(G5))-TODAY()) &amp; " Days" )</f>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
@@ -3947,25 +4232,25 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" s="45" t="s">
+      <c r="C6" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="str">
-        <f t="shared" ref="H6:H9" ca="1" si="0">IF(G6="", "", DATEDIF(G6, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G6, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I6" s="35" t="str">
-        <f ca="1">IF(G6="", "", IF(DATE(YEAR(TODAY()),MONTH(G6),DAY(G6))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G6),DAY(G6))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G6),DAY(G6))-TODAY()) &amp; " Days" )</f>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
@@ -3976,16 +4261,16 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="45" t="s">
+      <c r="C7" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="4"/>
@@ -3994,7 +4279,7 @@
         <v/>
       </c>
       <c r="I7" s="35" t="str">
-        <f t="shared" ref="I7:I9" ca="1" si="1">IF(G7="", "", IF(DATE(YEAR(TODAY()),MONTH(G7),DAY(G7))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G7),DAY(G7))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G7),DAY(G7))-TODAY()) &amp; " Days" )</f>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
@@ -4003,16 +4288,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>102</v>
+        <v>120</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>7</v>
@@ -4032,16 +4317,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>102</v>
+        <v>120</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>7</v>
@@ -4056,61 +4341,61 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="F10" s="46" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="str">
-        <f ca="1">IF(G10="", "", DATEDIF(G10, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G10, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I10" s="35" t="str">
-        <f ca="1">IF(G10="", "", IF(DATE(YEAR(TODAY()),MONTH(G10),DAY(G10))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G10),DAY(G10))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G10),DAY(G10))-TODAY()) &amp; " Days" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="str">
-        <f t="shared" ref="H11" ca="1" si="2">IF(G11="", "", DATEDIF(G11, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G11, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I11" s="35" t="str">
-        <f ca="1">IF(G11="", "", IF(DATE(YEAR(TODAY()),MONTH(G11),DAY(G11))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G11),DAY(G11))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G11),DAY(G11))-TODAY()) &amp; " Days" )</f>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
@@ -4119,27 +4404,27 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>9</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="str">
-        <f t="shared" ref="H12" ca="1" si="3">IF(G12="", "", DATEDIF(G12, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G12, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I12" s="35" t="str">
-        <f t="shared" ref="I12:I23" ca="1" si="4">IF(G12="", "", IF(DATE(YEAR(TODAY()),MONTH(G12),DAY(G12))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G12),DAY(G12))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G12),DAY(G12))-TODAY()) &amp; " Days" )</f>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
@@ -4148,27 +4433,27 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4" t="str">
-        <f t="shared" ref="H13" ca="1" si="5">IF(G13="", "", DATEDIF(G13, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G13, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I13" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
@@ -4177,27 +4462,27 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="str">
-        <f t="shared" ref="H14" ca="1" si="6">IF(G14="", "", DATEDIF(G14, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G14, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I14" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
@@ -4206,27 +4491,27 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>10</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4" t="str">
-        <f t="shared" ref="H15" ca="1" si="7">IF(G15="", "", DATEDIF(G15, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G15, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I15" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
@@ -4235,28 +4520,30 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="5">
+        <v>28239</v>
+      </c>
       <c r="H16" s="4" t="str">
-        <f t="shared" ref="H16" ca="1" si="8">IF(G16="", "", DATEDIF(G16, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G16, TODAY(), "YM") &amp; " months")</f>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>47 years, 9 months</v>
       </c>
       <c r="I16" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
+        <f ca="1">IF(G16="", "", IF(DATE(YEAR(TODAY()),MONTH(G16),DAY(G16))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G16),DAY(G16))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G16),DAY(G16))-TODAY()) &amp; " Days" )</f>
+        <v>67 Days</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4264,27 +4551,27 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>10</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4" t="str">
-        <f t="shared" ref="H17" ca="1" si="9">IF(G17="", "", DATEDIF(G17, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G17, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I17" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">IF(G17="", "", IF(DATE(YEAR(TODAY()),MONTH(G17),DAY(G17))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G17),DAY(G17))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G17),DAY(G17))-TODAY()) &amp; " Days" )</f>
         <v/>
       </c>
     </row>
@@ -4293,27 +4580,27 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4" t="str">
-        <f t="shared" ref="H18" ca="1" si="10">IF(G18="", "", DATEDIF(G18, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G18, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I18" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="I18:I47" ca="1" si="2">IF(G18="", "", IF(DATE(YEAR(TODAY()),MONTH(G18),DAY(G18))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G18),DAY(G18))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G18),DAY(G18))-TODAY()) &amp; " Days" )</f>
         <v/>
       </c>
     </row>
@@ -4322,27 +4609,27 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4" t="str">
-        <f t="shared" ref="H19" ca="1" si="11">IF(G19="", "", DATEDIF(G19, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G19, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I19" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4351,27 +4638,27 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4" t="str">
-        <f t="shared" ref="H20" ca="1" si="12">IF(G20="", "", DATEDIF(G20, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G20, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I20" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4380,27 +4667,27 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>11</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="str">
-        <f t="shared" ref="H21" ca="1" si="13">IF(G21="", "", DATEDIF(G21, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G21, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I21" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4409,27 +4696,27 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>11</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4" t="str">
-        <f t="shared" ref="H22" ca="1" si="14">IF(G22="", "", DATEDIF(G22, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G22, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I22" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4438,27 +4725,27 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>11</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="str">
-        <f t="shared" ref="H23" ca="1" si="15">IF(G23="", "", DATEDIF(G23, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G23, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I23" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4467,30 +4754,28 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>11</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="5">
-        <v>28239</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="4"/>
       <c r="H24" s="4" t="str">
-        <f t="shared" ref="H24" ca="1" si="16">IF(G24="", "", DATEDIF(G24, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G24, TODAY(), "YM") &amp; " months")</f>
-        <v>47 years, 9 months</v>
+        <f t="shared" ca="1" si="0"/>
+        <v/>
       </c>
       <c r="I24" s="35" t="str">
-        <f ca="1">IF(G24="", "", IF(DATE(YEAR(TODAY()),MONTH(G24),DAY(G24))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G24),DAY(G24))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G24),DAY(G24))-TODAY()) &amp; " Days" )</f>
-        <v>67 Days</v>
+        <f t="shared" ca="1" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4498,27 +4783,27 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>11</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" s="14" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4" t="str">
-        <f t="shared" ref="H25" ca="1" si="17">IF(G25="", "", DATEDIF(G25, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G25, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I25" s="35" t="str">
-        <f ca="1">IF(G25="", "", IF(DATE(YEAR(TODAY()),MONTH(G25),DAY(G25))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G25),DAY(G25))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G25),DAY(G25))-TODAY()) &amp; " Days" )</f>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4527,27 +4812,27 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>11</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4" t="str">
-        <f t="shared" ref="H26" ca="1" si="18">IF(G26="", "", DATEDIF(G26, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G26, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I26" s="35" t="str">
-        <f t="shared" ref="I26:I55" ca="1" si="19">IF(G26="", "", IF(DATE(YEAR(TODAY()),MONTH(G26),DAY(G26))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G26),DAY(G26))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G26),DAY(G26))-TODAY()) &amp; " Days" )</f>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4556,27 +4841,27 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>11</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4" t="str">
-        <f t="shared" ref="H27" ca="1" si="20">IF(G27="", "", DATEDIF(G27, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G27, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I27" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4585,27 +4870,27 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>11</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4" t="str">
-        <f t="shared" ref="H28" ca="1" si="21">IF(G28="", "", DATEDIF(G28, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G28, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I28" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4614,27 +4899,27 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>12</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4" t="str">
-        <f t="shared" ref="H29" ca="1" si="22">IF(G29="", "", DATEDIF(G29, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G29, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I29" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4643,27 +4928,27 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>12</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4" t="str">
-        <f t="shared" ref="H30" ca="1" si="23">IF(G30="", "", DATEDIF(G30, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G30, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I30" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4672,27 +4957,27 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>12</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4" t="str">
-        <f t="shared" ref="H31" ca="1" si="24">IF(G31="", "", DATEDIF(G31, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G31, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I31" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4701,27 +4986,27 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>12</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="str">
-        <f t="shared" ref="H32" ca="1" si="25">IF(G32="", "", DATEDIF(G32, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G32, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I32" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4730,27 +5015,27 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>13</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="str">
-        <f t="shared" ref="H33" ca="1" si="26">IF(G33="", "", DATEDIF(G33, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G33, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I33" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4759,27 +5044,27 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>13</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4" t="str">
-        <f t="shared" ref="H34" ca="1" si="27">IF(G34="", "", DATEDIF(G34, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G34, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I34" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4788,27 +5073,27 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>13</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F35" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4" t="str">
-        <f t="shared" ref="H35" ca="1" si="28">IF(G35="", "", DATEDIF(G35, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G35, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I35" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4817,27 +5102,27 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>13</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4" t="str">
-        <f t="shared" ref="H36" ca="1" si="29">IF(G36="", "", DATEDIF(G36, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G36, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I36" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4846,27 +5131,27 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>13</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F37" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4" t="str">
-        <f t="shared" ref="H37:H100" ca="1" si="30">IF(G37="", "", DATEDIF(G37, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G37, TODAY(), "YM") &amp; " months")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I37" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4875,27 +5160,27 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>13</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F38" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I38" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4904,27 +5189,27 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>14</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I39" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4933,27 +5218,27 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>14</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F40" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F40" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I40" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4962,27 +5247,27 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>14</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F41" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I41" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -4991,27 +5276,27 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>14</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F42" s="16" t="s">
         <v>7</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I42" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -5020,27 +5305,27 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>14</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>7</v>
+        <v>7</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I43" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -5049,27 +5334,27 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>44</v>
+        <v>164</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>9</v>
+        <v>127</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I44" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -5078,27 +5363,27 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>9</v>
+        <v>127</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I45" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -5107,27 +5392,27 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>9</v>
+        <v>127</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I46" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -5136,27 +5421,27 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>15</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F47" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F47" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I47" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
@@ -5165,28 +5450,30 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>15</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="5">
+        <v>29258</v>
+      </c>
       <c r="H48" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>45 years, 0 months</v>
       </c>
       <c r="I48" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
-        <v/>
+        <f ca="1">IF(G48="", "", IF(DATE(YEAR(TODAY()),MONTH(G48),DAY(G48))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G48),DAY(G48))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G48),DAY(G48))-TODAY()) &amp; " Days" )</f>
+        <v>356 Days</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5194,27 +5481,27 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>15</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F49" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F49" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I49" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f ca="1">IF(G49="", "", IF(DATE(YEAR(TODAY()),MONTH(G49),DAY(G49))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G49),DAY(G49))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G49),DAY(G49))-TODAY()) &amp; " Days" )</f>
         <v/>
       </c>
     </row>
@@ -5223,27 +5510,27 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>15</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F50" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F50" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I50" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ref="I50:I61" ca="1" si="3">IF(G50="", "", IF(DATE(YEAR(TODAY()),MONTH(G50),DAY(G50))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G50),DAY(G50))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G50),DAY(G50))-TODAY()) &amp; " Days" )</f>
         <v/>
       </c>
     </row>
@@ -5252,28 +5539,30 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>15</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F51" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="5">
+        <v>33562</v>
+      </c>
       <c r="H51" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>33 years, 2 months</v>
       </c>
       <c r="I51" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>277 Days</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5281,28 +5570,30 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>16</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D52" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52" s="4"/>
+      <c r="C52" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="5">
+        <v>34480</v>
+      </c>
       <c r="H52" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>30 years, 8 months</v>
       </c>
       <c r="I52" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>99 Days</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5310,28 +5601,30 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>16</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53" s="4"/>
+      <c r="C53" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="5">
+        <v>36484</v>
+      </c>
       <c r="H53" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>25 years, 2 months</v>
       </c>
       <c r="I53" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>277 Days</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5339,27 +5632,27 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>16</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F54" s="8" t="s">
+      <c r="C54" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F54" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I54" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
     </row>
@@ -5368,27 +5661,27 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>16</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F55" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F55" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="I55" s="35" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
     </row>
@@ -5397,30 +5690,28 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>19</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G56" s="5">
-        <v>29258</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="4"/>
       <c r="H56" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>45 years, 0 months</v>
+        <f t="shared" ca="1" si="0"/>
+        <v/>
       </c>
       <c r="I56" s="35" t="str">
-        <f ca="1">IF(G56="", "", IF(DATE(YEAR(TODAY()),MONTH(G56),DAY(G56))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G56),DAY(G56))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G56),DAY(G56))-TODAY()) &amp; " Days" )</f>
-        <v>356 Days</v>
+        <f t="shared" ca="1" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="57" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5428,28 +5719,30 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>19</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G57" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="5">
+        <v>34511</v>
+      </c>
       <c r="H57" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>30 years, 7 months</v>
       </c>
       <c r="I57" s="35" t="str">
-        <f ca="1">IF(G57="", "", IF(DATE(YEAR(TODAY()),MONTH(G57),DAY(G57))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G57),DAY(G57))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G57),DAY(G57))-TODAY()) &amp; " Days" )</f>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>130 Days</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5457,28 +5750,30 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>19</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G58" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="5">
+        <v>35744</v>
+      </c>
       <c r="H58" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>27 years, 3 months</v>
       </c>
       <c r="I58" s="35" t="str">
-        <f t="shared" ref="I58:I69" ca="1" si="31">IF(G58="", "", IF(DATE(YEAR(TODAY()),MONTH(G58),DAY(G58))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G58),DAY(G58))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G58),DAY(G58))-TODAY()) &amp; " Days" )</f>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>267 Days</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5486,30 +5781,30 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>19</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F59" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F59" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G59" s="5">
-        <v>33562</v>
+        <v>36426</v>
       </c>
       <c r="H59" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>33 years, 2 months</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>25 years, 4 months</v>
       </c>
       <c r="I59" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v>277 Days</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>219 Days</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5517,30 +5812,28 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>19</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" s="5">
-        <v>34480</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="4"/>
       <c r="H60" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>30 years, 8 months</v>
+        <f t="shared" ca="1" si="0"/>
+        <v/>
       </c>
       <c r="I60" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v>99 Days</v>
+        <f t="shared" ca="1" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="61" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5548,30 +5841,28 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>19</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G61" s="5">
-        <v>36484</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="4"/>
       <c r="H61" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>25 years, 2 months</v>
+        <f t="shared" ca="1" si="0"/>
+        <v/>
       </c>
       <c r="I61" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v>277 Days</v>
+        <f t="shared" ca="1" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="62" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5579,28 +5870,30 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>19</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G62" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="5">
+        <v>36968</v>
+      </c>
       <c r="H62" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>23 years, 10 months</v>
       </c>
       <c r="I62" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v/>
+        <f ca="1">IF(G62="", "", IF(DATE(YEAR(TODAY()),MONTH(G62),DAY(G62))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G62),DAY(G62))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G62),DAY(G62))-TODAY()) &amp; " Days" )</f>
+        <v>30 Days</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5608,28 +5901,30 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>20</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E63" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F63" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G63" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="5">
+        <v>37785</v>
+      </c>
       <c r="H63" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>21 years, 8 months</v>
       </c>
       <c r="I63" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v/>
+        <f ca="1">IF(G63="", "", IF(DATE(YEAR(TODAY()),MONTH(G63),DAY(G63))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G63),DAY(G63))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G63),DAY(G63))-TODAY()) &amp; " Days" )</f>
+        <v>117 Days</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5637,28 +5932,30 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>20</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F64" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G64" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" s="5">
+        <v>39043</v>
+      </c>
       <c r="H64" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="0"/>
+        <v>18 years, 2 months</v>
       </c>
       <c r="I64" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v/>
+        <f t="shared" ref="I64:I94" ca="1" si="4">IF(G64="", "", IF(DATE(YEAR(TODAY()),MONTH(G64),DAY(G64))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G64),DAY(G64))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G64),DAY(G64))-TODAY()) &amp; " Days" )</f>
+        <v>279 Days</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5666,30 +5963,30 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>20</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E65" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F65" s="18" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="G65" s="5">
-        <v>34511</v>
+        <v>40162</v>
       </c>
       <c r="H65" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>30 years, 7 months</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>15 years, 2 months</v>
       </c>
       <c r="I65" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v>130 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>302 Days</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5697,30 +5994,30 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>20</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F66" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F66" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G66" s="5">
-        <v>35744</v>
+        <v>42678</v>
       </c>
       <c r="H66" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>27 years, 3 months</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8 years, 3 months</v>
       </c>
       <c r="I66" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v>267 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>261 Days</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5728,30 +6025,30 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>20</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F67" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="F67" s="20" t="s">
         <v>7</v>
       </c>
       <c r="G67" s="5">
-        <v>36426</v>
+        <v>37602</v>
       </c>
       <c r="H67" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>25 years, 4 months</v>
+        <f t="shared" ref="H67:H94" ca="1" si="5">IF(G67="", "", DATEDIF(G67, TODAY(), "Y") &amp; " years, " &amp; DATEDIF(G67, TODAY(), "YM") &amp; " months")</f>
+        <v>22 years, 2 months</v>
       </c>
       <c r="I67" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v>219 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>299 Days</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5759,28 +6056,30 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>20</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F68" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G68" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="C68" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68" s="5">
+        <v>39049</v>
+      </c>
       <c r="H68" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="5"/>
+        <v>18 years, 2 months</v>
       </c>
       <c r="I68" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>285 Days</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5788,28 +6087,30 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>20</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F69" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G69" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="5">
+        <v>39877</v>
+      </c>
       <c r="H69" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
+        <f t="shared" ca="1" si="5"/>
+        <v>15 years, 11 months</v>
       </c>
       <c r="I69" s="35" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>17 Days</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5817,30 +6118,30 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>22</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F70" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="F70" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G70" s="5">
-        <v>36968</v>
+        <v>40931</v>
       </c>
       <c r="H70" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>23 years, 10 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>13 years, 0 months</v>
       </c>
       <c r="I70" s="35" t="str">
-        <f ca="1">IF(G70="", "", IF(DATE(YEAR(TODAY()),MONTH(G70),DAY(G70))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G70),DAY(G70))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G70),DAY(G70))-TODAY()) &amp; " Days" )</f>
-        <v>30 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>341 Days</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5848,30 +6149,30 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>22</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D71" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E71" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F71" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="F71" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G71" s="5">
-        <v>37785</v>
+        <v>44379</v>
       </c>
       <c r="H71" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>21 years, 8 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3 years, 7 months</v>
       </c>
       <c r="I71" s="35" t="str">
-        <f ca="1">IF(G71="", "", IF(DATE(YEAR(TODAY()),MONTH(G71),DAY(G71))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G71),DAY(G71))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G71),DAY(G71))-TODAY()) &amp; " Days" )</f>
-        <v>117 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>136 Days</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5879,30 +6180,28 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>22</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D72" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F72" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G72" s="5">
-        <v>39043</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C72" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F72" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G72" s="4"/>
       <c r="H72" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>18 years, 2 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I72" s="35" t="str">
-        <f t="shared" ref="I72:I100" ca="1" si="32">IF(G72="", "", IF(DATE(YEAR(TODAY()),MONTH(G72),DAY(G72))&gt;=TODAY(), DATE(YEAR(TODAY()),MONTH(G72),DAY(G72))-TODAY(), DATE(YEAR(TODAY())+1,MONTH(G72),DAY(G72))-TODAY()) &amp; " Days" )</f>
-        <v>279 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="73" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5910,30 +6209,28 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>22</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D73" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E73" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F73" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G73" s="5">
-        <v>40162</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E73" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" s="4"/>
       <c r="H73" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>15 years, 2 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I73" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>302 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="74" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5941,30 +6238,28 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>22</v>
-      </c>
-      <c r="C74" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D74" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F74" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G74" s="5">
-        <v>42678</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C74" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D74" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" s="4"/>
       <c r="H74" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>8 years, 3 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I74" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>261 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="75" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5972,30 +6267,28 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>23</v>
-      </c>
-      <c r="C75" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D75" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E75" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G75" s="5">
-        <v>37602</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C75" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D75" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G75" s="4"/>
       <c r="H75" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>22 years, 2 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I75" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>299 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="76" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6003,30 +6296,28 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>23</v>
-      </c>
-      <c r="C76" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E76" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F76" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G76" s="5">
-        <v>39049</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C76" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="D76" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G76" s="4"/>
       <c r="H76" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>18 years, 2 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I76" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>285 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="77" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6034,30 +6325,28 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>23</v>
-      </c>
-      <c r="C77" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E77" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F77" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G77" s="5">
-        <v>39877</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="D77" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E77" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77" s="4"/>
       <c r="H77" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>15 years, 11 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I77" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>17 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="78" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6065,30 +6354,28 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>23</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="D78" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E78" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F78" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G78" s="5">
-        <v>40931</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C78" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="D78" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E78" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G78" s="4"/>
       <c r="H78" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>13 years, 0 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I78" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>341 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="79" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6096,30 +6383,28 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>23</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D79" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E79" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F79" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G79" s="5">
-        <v>44379</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C79" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="D79" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="E79" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="F79" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="4"/>
       <c r="H79" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>3 years, 7 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I79" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>136 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="80" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6127,27 +6412,27 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>27</v>
-      </c>
-      <c r="C80" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D80" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E80" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F80" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C80" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="D80" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="E80" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="F80" s="26" t="s">
         <v>7</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="I80" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
@@ -6156,27 +6441,27 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>27</v>
-      </c>
-      <c r="C81" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D81" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E81" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F81" s="22" t="s">
-        <v>7</v>
+        <v>49</v>
+      </c>
+      <c r="C81" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="D81" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="E81" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="F81" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="I81" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
@@ -6185,27 +6470,27 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>55</v>
-      </c>
-      <c r="C82" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D82" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E82" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F82" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D82" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="E82" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="F82" s="26" t="s">
         <v>7</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="I82" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
@@ -6214,30 +6499,28 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>55</v>
-      </c>
-      <c r="C83" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D83" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E83" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F83" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G83" s="4">
-        <v>38779</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F83" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G83" s="4"/>
       <c r="H83" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>18 years, 11 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I83" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>15 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="84" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6245,30 +6528,30 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>55</v>
-      </c>
-      <c r="C84" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D84" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E84" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F84" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G84" s="4">
-        <v>40171</v>
+        <v>50</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F84" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G84" s="5">
+        <v>45292</v>
       </c>
       <c r="H84" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>15 years, 1 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1 years, 1 months</v>
       </c>
       <c r="I84" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>311 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>319 Days</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6276,30 +6559,30 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>55</v>
-      </c>
-      <c r="C85" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D85" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E85" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F85" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G85" s="4">
-        <v>40850</v>
+        <v>54</v>
+      </c>
+      <c r="C85" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="D85" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="E85" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="F85" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G85" s="5">
+        <v>44214</v>
       </c>
       <c r="H85" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>13 years, 3 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>4 years, 0 months</v>
       </c>
       <c r="I85" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>260 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>336 Days</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6309,28 +6592,26 @@
       <c r="B86">
         <v>55</v>
       </c>
-      <c r="C86" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D86" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E86" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F86" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G86" s="4">
-        <v>41978</v>
-      </c>
+      <c r="C86" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D86" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="E86" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F86" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G86" s="4"/>
       <c r="H86" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>10 years, 2 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I86" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>292 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="87" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6338,30 +6619,30 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>57</v>
-      </c>
-      <c r="C87" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D87" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E87" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="F87" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G87" s="4">
-        <v>39801</v>
+        <v>55</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="D87" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="E87" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F87" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G87" s="5">
+        <v>43848</v>
       </c>
       <c r="H87" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>16 years, 1 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5 years, 0 months</v>
       </c>
       <c r="I87" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>306 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>336 Days</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6369,30 +6650,30 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>57</v>
-      </c>
-      <c r="C88" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D88" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E88" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="F88" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G88" s="4">
-        <v>40850</v>
+        <v>55</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F88" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G88" s="5">
+        <v>43848</v>
       </c>
       <c r="H88" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>13 years, 3 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5 years, 0 months</v>
       </c>
       <c r="I88" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>260 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>336 Days</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6400,27 +6681,27 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>57</v>
-      </c>
-      <c r="C89" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D89" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E89" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="F89" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D89" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E89" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F89" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="I89" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
@@ -6429,27 +6710,27 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>57</v>
-      </c>
-      <c r="C90" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D90" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E90" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="F90" s="26" t="s">
-        <v>7</v>
+        <v>38</v>
+      </c>
+      <c r="C90" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="D90" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E90" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F90" s="30" t="s">
+        <v>13</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="I90" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
@@ -6458,30 +6739,28 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>58</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E91" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F91" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G91" s="4">
-        <v>43397</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C91" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D91" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="E91" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="F91" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G91" s="4"/>
       <c r="H91" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>6 years, 3 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I91" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>250 Days</v>
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="92" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6489,298 +6768,93 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>58</v>
-      </c>
-      <c r="C92" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D92" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E92" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F92" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G92" s="5">
-        <v>45292</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E92" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="F92" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" s="6"/>
       <c r="H92" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>1 years, 1 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="I92" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>319 Days</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93">
-        <v>62</v>
-      </c>
-      <c r="C93" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D93" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="E93" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="F93" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="G93" s="5">
-        <v>44214</v>
+        <v>58</v>
+      </c>
+      <c r="C93" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="D93" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="E93" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="F93" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G93" s="36">
+        <v>45394</v>
       </c>
       <c r="H93" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>4 years, 0 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0 years, 10 months</v>
       </c>
       <c r="I93" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>336 Days</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <f t="shared" ca="1" si="4"/>
+        <v>55 Days</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94">
-        <v>63</v>
-      </c>
-      <c r="C94" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D94" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E94" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F94" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G94" s="4">
-        <v>43389</v>
+        <v>57</v>
+      </c>
+      <c r="C94" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="D94" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="E94" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="F94" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" s="36">
+        <v>45516</v>
       </c>
       <c r="H94" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>6 years, 4 months</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0 years, 6 months</v>
       </c>
       <c r="I94" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>242 Days</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="B95">
-        <v>63</v>
-      </c>
-      <c r="C95" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="D95" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E95" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F95" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G95" s="5">
-        <v>43848</v>
-      </c>
-      <c r="H95" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>5 years, 0 months</v>
-      </c>
-      <c r="I95" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>336 Days</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>95</v>
-      </c>
-      <c r="B96">
-        <v>46</v>
-      </c>
-      <c r="C96" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D96" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E96" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="F96" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="I96" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97">
-        <v>96</v>
-      </c>
-      <c r="B97">
-        <v>46</v>
-      </c>
-      <c r="C97" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="D97" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E97" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="F97" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="I97" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98">
-        <v>97</v>
-      </c>
-      <c r="B98">
-        <v>49</v>
-      </c>
-      <c r="C98" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="D98" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="E98" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="F98" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="I98" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99">
-        <v>98</v>
-      </c>
-      <c r="B99">
-        <v>42</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E99" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="F99" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="I99" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>99</v>
-      </c>
-      <c r="B100">
-        <v>66</v>
-      </c>
-      <c r="C100" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="D100" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E100" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="F100" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G100" s="5">
-        <v>45394</v>
-      </c>
-      <c r="H100" s="4" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v>0 years, 10 months</v>
-      </c>
-      <c r="I100" s="35" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v>55 Days</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G101"/>
-    </row>
-    <row r="102" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G102"/>
-    </row>
-    <row r="103" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G103"/>
-    </row>
-    <row r="104" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G104"/>
-    </row>
-    <row r="105" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G105"/>
-    </row>
-    <row r="106" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G106"/>
-    </row>
-    <row r="107" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G107"/>
-    </row>
-    <row r="108" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G108"/>
+        <f t="shared" ca="1" si="4"/>
+        <v>177 Days</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>